<commit_message>
conditional formatting for number of matches
</commit_message>
<xml_diff>
--- a/inputExample.xlsx
+++ b/inputExample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MA\PycharmProjects\automation3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MA\PycharmProjects\Matrix1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A26086-7EEE-4CED-8B81-1756F61102F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0679270-AEDA-4E4A-BC19-A20CBEE98FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1714,6 +1714,9 @@
       <c r="D25" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6">
@@ -1896,6 +1899,9 @@
       </c>
       <c r="D30" s="7" t="s">
         <v>24</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -1959,6 +1965,9 @@
       </c>
       <c r="D32" s="7" t="s">
         <v>24</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
       </c>
       <c r="F32" s="6">
         <v>1</v>

</xml_diff>